<commit_message>
Added issues to the Issue List.xlsx Change the color of the RegisterPage.xaml register button Change the android package name to com.micronians.rideshare
</commit_message>
<xml_diff>
--- a/docs/Issue List.xlsx
+++ b/docs/Issue List.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\RideShareRepository\trunk\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="5100"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="50">
   <si>
     <t>Login Page</t>
   </si>
@@ -27,9 +32,6 @@
     <t>Pre populate country code and provide in a drop dowon(Minor)</t>
   </si>
   <si>
-    <t>Mobile Number validation does not work properly(Major)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Select profile image button is not User Friendly, User tries to click the </t>
   </si>
   <si>
@@ -106,13 +108,168 @@
   </si>
   <si>
     <t>Menu</t>
+  </si>
+  <si>
+    <t>Register Page/Edit Profile</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Need to show the flag + Country name in the country code picking section of the phone number as the user experience is not good. Might need to change the control to a ListView from a picker. Refer to the Uber country code viewer. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+https://developer.xamarin.com/api/type/Xamarin.Forms.ListView/</t>
+    </r>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>ReOpened</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>java.lang.RuntimeException: java.lang.reflect.InvocationTargetException
+ at com.android.internal.os.ZygoteInit.main(ZygoteInit.java:1120)
+Caused by: java.lang.reflect.InvocationTargetException
+ at java.lang.reflect.Method.invoke(Native Method)
+ at com.android.internal.os.ZygoteInit$MethodAndArgsCaller.run(ZygoteInit.java:1230)
+ ... 1 more
+Caused by: android.runtime.JavaProxyThrowable: System.ArgumentOutOfRangeException: Index was out of range. Must be non-negative and less than the size of the collection.
+Parameter name: index
+  at System.ThrowHelper.ThrowArgumentOutOfRangeException (ExceptionArgument argument, ExceptionResource resource) &lt;0x92db0140 + 0x00038&gt; in &lt;filename unknown&gt;:0 
+  at System.ThrowHelper.ThrowArgumentOutOfRangeException () &lt;0x92db0118 + 0x0000f&gt; in &lt;filename unknown&gt;:0 
+  at System.Collections.Generic.List`1[T].get_Item (Int32 index) &lt;0xb32143f8 + 0x00027&gt; in &lt;filename unknown&gt;:0 
+  at System.Collections.ObjectModel.Collection`1[T].get_Item (Int32 index) &lt;0xa8928d78 + 0x00047&gt; in &lt;filename unknown&gt;:0 
+  at RideShare.RegisterPage.MobileNumberValidator () &lt;0x92dafc58 + 0x00087&gt; in &lt;filename unknown&gt;:0 
+  at RideShare.RegisterPage.mobileNumberEntry_Unfocused (System.Object sender, Xamarin.Forms.FocusEventArgs e) &lt;0x92dafba8 + 0x00063&gt; in &lt;filename unknown&gt;:0 
+  at Xamarin.Forms.VisualElement.OnUnfocus () &lt;0x92dafaa8 + 0x0004b&gt; in &lt;filename unknown&gt;:0 
+  at Xamarin.Forms.VisualElement.OnIsFocusedPropertyChanged (Xamarin.Forms.BindableObject bindable, System.Object oldvalue, System.Object newvalue) &lt;0x92dae000 + 0x000a3&gt; in &lt;filename unknown&gt;:0 
+  at Xamarin.Forms.BindableObject.SetValueActual (Xamarin.Forms.BindableProperty property, Xamarin.Forms.BindablePropertyContext context, System.Object value, Boolean currentlyApplying, SetValueFlags attributes, Boolean silent) &lt;0xaeadebd0 + 0x0029f&gt; in &lt;filename unknown&gt;:0 
+  at Xamarin.Forms.BindableObject.SetValueCore (Xamarin.Forms.BindableProperty property, System.Object value, SetValueFlags attributes, SetValuePrivateFlags privateAttributes) &lt;0xaeadd5e8 + 0x002eb&gt; in &lt;filename unknown&gt;:0 
+  at Xamarin.Forms.BindableObject.SetValueCore (Xamarin.Forms.BindablePropertyKey propertyKey, System.Object value, SetValueFlags attributes) &lt;0x935bdad0 + 0x0003b&gt; in &lt;filename unknown&gt;:0 
+  at Xamarin.Forms.Element.Xamarin.Forms.IElementController.SetValueFromRenderer (Xamarin.Forms.BindablePropertyKey property, System.Object value) &lt;0x935bda78 + 0x00027&gt; in &lt;filename unknown&gt;:0 
+  at Xamarin.Forms.Platform.Android.ViewRenderer`2[TView,TNativeView].Android.Views.View.IOnFocusChangeListener.OnFocusChange (Android.Views.View v, Boolean hasFocus) &lt;0x939d5b50 + 0x002e7&gt; in &lt;filename unknown&gt;:0 
+  at Android.Views.View+IOnFocusChangeListenerInvoker.n_OnFocusChange_Landroid_view_View_Z (IntPtr jnienv, IntPtr native__this, IntPtr native_v, Boolean hasFocus) &lt;0x939d5aa8 + 0x0006b&gt; in &lt;filename unknown&gt;:0 
+  at (wrapper dynamic-method) System.Object:ad85bd3a-d308-4a45-af1b-34295de771c5 (intptr,intptr,intptr,bool)
+--- End of stack trace from previous location where exception was thrown ---
+  at System.Runtime.ExceptionServices.ExceptionDispatchInfo.Throw () &lt;0x92db4928 + 0x00024&gt; in &lt;filename unknown&gt;:0 
+  at Java.Interop.JniEnvironment+InstanceMethods.CallVoidMethod (JniObjectReference instance, Java.Interop.JniMethodInfo method, Java.Interop.JniArgumentValue* args) &lt;0xaeb392b8 + 0x000af&gt; in &lt;filename unknown&gt;:0 
+  at Java.Interop.JniPeerMembers+JniInstanceMethods.InvokeVirtualVoidMethod (System.String encodedMember, IJavaPeerable self, Java.Interop.JniArgumentValue* parameters) &lt;0xb31dfb78 + 0x00087&gt; in &lt;filename unknown&gt;:0 
+  at Android.Views.View.ClearFocus () &lt;0x92daf9f0 + 0x00043&gt; in &lt;filename unknown&gt;:0 
+  at Xamarin.Forms.Platform.Android.PlatformRenderer.DispatchTouchEvent (Android.Views.MotionEvent e) &lt;0x92ea3a70 + 0x0065b&gt; in &lt;filename unknown&gt;:0 
+  at Android.Views.View.n_DispatchTouchEvent_Landroid_view_MotionEvent_ (IntPtr jnienv, IntPtr native__this, IntPtr native_e) &lt;0x92ea3858 + 0x0005b&gt; in &lt;filename unknown&gt;:0 
+  at (wrapper dynamic-method) System.Object:5e195528-53f3-4de5-acaf-1ea83fa9e0c9 (intptr,intptr,intptr)
+ at md5b60ffeb829f638581ab2bb9b1a7f4f3f.PlatformRenderer.n_dispatchTouchEvent(Native Method)
+ at md5b60ffeb829f638581ab2bb9b1a7f4f3f.PlatformRenderer.dispatchTouchEvent(PlatformRenderer.java:47)
+ at android.view.ViewGroup.dispatchTransformedTouchEvent(ViewGroup.java:2841)
+ at android.view.ViewGroup.dispatchTouchEvent(ViewGroup.java:2516)
+ at android.view.ViewGroup.dispatchTransformedTouchEvent(ViewGroup.java:2841)
+ at android.view.ViewGroup.dispatchTouchEvent(ViewGroup.java:2516)
+ at android.view.ViewGroup.dispatchTransformedTouchEvent(ViewGroup.java:2841)
+ at android.view.ViewGroup.dispatchTouchEvent(ViewGroup.java:2516)
+ at android.view.ViewGroup.dispatchTransformedTouchEvent(ViewGroup.java:2841)
+ at android.view.ViewGroup.dispatchTouchEvent(ViewGroup.java:2516)
+ at com.android.internal.policy.PhoneWindow$DecorView.superDispatchTouchEvent(PhoneWindow.java:2795)
+ at com.android.internal.policy.PhoneWindow.superDispatchTouchEvent(PhoneWindow.java:1848)
+ at android.app.Activity.dispatchTouchEvent(Activity.java:3047)
+ at com.android.internal.policy.PhoneWindow$DecorView.dispatchTouchEvent(PhoneWindow.java:2756)
+ at android.view.View.dispatchPointerEvent(View.java:10229)
+ at android.view.ViewRootImpl$ViewPostImeInputStage.processPointerEvent(ViewRootImpl.java:5357)
+ at android.view.ViewRootImpl$ViewPostImeInputStage.onProcess(ViewRootImpl.java:5193)
+ at android.view.ViewRootImpl$InputStage.deliver(ViewRootImpl.java:4633)
+ at android.view.ViewRootImpl$InputStage.onDeliverToNext(ViewRootImpl.java:4686)
+ at android.view.ViewRootImpl$InputStage.forward(ViewRootImpl.java:4652)
+ at android.view.ViewRootImpl$AsyncInputStage.forward(ViewRootImpl.java:4794)
+ at android.view.ViewRootImpl$InputStage.apply(ViewRootImpl.java:4660)
+ at android.view.ViewRootImpl$AsyncInputStage.apply(ViewRootImpl.java:4851)
+ at android.view.ViewRootImpl$InputStage.deliver(ViewRootImpl.java:4633)
+ at android.view.ViewRootImpl$InputStage.onDeliverToNext(ViewRootImpl.java:4686)
+ at android.view.ViewRootImpl$InputStage.forward(ViewRootImpl.java:4652)
+ at android.view.ViewRootImpl$InputStage.apply(ViewRootImpl.java:4660)
+ at android.view.ViewRootImpl$InputStage.deliver(ViewRootImpl.java:4633)
+ at android.view.ViewRootImpl.deliverInputEvent(ViewRootImpl.java:7330)
+ at android.view.ViewRootImpl.doProcessInputEvents(ViewRootImpl.java:7208)
+ at android.view.ViewRootImpl.enqueueInputEvent(ViewRootImpl.java:7169)
+ at android.view.ViewRootImpl$WindowInputEventReceiver.onInputEvent(ViewRootImpl.java:7440)
+ at android.view.InputEventReceiver.dispatchInputEvent(InputEventReceiver.java:185)
+ at android.os.MessageQueue.nativePollOnce(Native Method)
+ at android.os.MessageQueue.next(MessageQueue.java:323)
+ at android.os.Looper.loop(Looper.java:143)
+ at android.app.ActivityThread.main(ActivityThread.java:7231)</t>
+  </si>
+  <si>
+    <t>Major</t>
+  </si>
+  <si>
+    <t>Mobile Number validation does not work properly(Major)
+The application crashed 3 times. It seems there is an index out of bounds exception in the mobile number validator. Refer details for log</t>
+  </si>
+  <si>
+    <t>When the application is closed, need to always sign in. Which is a bad user experience</t>
+  </si>
+  <si>
+    <t>Even after Dimuth cleared his application data, it shows an old user name pre-populated as the user name</t>
+  </si>
+  <si>
+    <t>Orphaned Data</t>
+  </si>
+  <si>
+    <t>Test data, several of Sithira's users appear on the map all the time</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>About Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Include Application Version </t>
+  </si>
+  <si>
+    <t>Map</t>
+  </si>
+  <si>
+    <t>Try to set the current location in the map, so that it loads that first as apposed to loading Rome and then navigating</t>
+  </si>
+  <si>
+    <t>Getting a ride</t>
+  </si>
+  <si>
+    <t>Selecting a driver to request a ride is not very intutive, may be we might need a button like "Request Ride" on that popup</t>
+  </si>
+  <si>
+    <t>User Experience</t>
+  </si>
+  <si>
+    <t>Functional</t>
+  </si>
+  <si>
+    <t>Riders and Drivers don't seem to get updated on the map at times</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,8 +285,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,8 +314,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -166,17 +350,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -447,7 +677,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -455,281 +685,432 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="84.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.5703125" customWidth="1"/>
+    <col min="2" max="2" width="84.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="38.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="D3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="B4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="B5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="3" t="s">
+      <c r="B9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="C13" s="6"/>
+      <c r="D13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="10"/>
+    </row>
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B14" r:id="rId1" display="https://developer.xamarin.com/api/type/Xamarin.Forms.ListView/"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Set the map location to user's current location and updated the issue list
</commit_message>
<xml_diff>
--- a/docs/Issue List.xlsx
+++ b/docs/Issue List.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\RideShareRepository\trunk\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="5100"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="61">
   <si>
     <t>Login Page</t>
   </si>
@@ -279,6 +284,18 @@
   </si>
   <si>
     <t>When a user registers for the first time, the device id will also be stored along with the user details. When the user tries to log in again, the user id will be retreived from that device id. This is for a better user experience.</t>
+  </si>
+  <si>
+    <t>Set the current user location at map init and commented out a section of code that prevented negative lat and long from loading</t>
+  </si>
+  <si>
+    <t>Nishantha</t>
+  </si>
+  <si>
+    <t>App consumes a lot of data</t>
+  </si>
+  <si>
+    <t>Critical</t>
   </si>
 </sst>
 </file>
@@ -444,9 +461,7 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -455,9 +470,7 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -491,15 +504,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -520,6 +524,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -794,7 +807,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -802,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -816,7 +829,7 @@
     <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="38.85546875" customWidth="1"/>
+    <col min="7" max="7" width="47.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
@@ -838,7 +851,7 @@
       <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>31</v>
       </c>
     </row>
@@ -859,7 +872,7 @@
       <c r="F2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="6"/>
+      <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -878,7 +891,7 @@
       <c r="F3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="6"/>
+      <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -897,24 +910,24 @@
       <c r="F4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="6"/>
+      <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="19"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
@@ -933,7 +946,7 @@
       <c r="F6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="6"/>
+      <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:8" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -973,7 +986,7 @@
       <c r="F8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="6"/>
+      <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
@@ -992,7 +1005,7 @@
       <c r="F9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="6"/>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
@@ -1009,7 +1022,7 @@
       <c r="F10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="6"/>
+      <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
@@ -1026,7 +1039,7 @@
       <c r="F11" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="6"/>
+      <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
@@ -1043,7 +1056,7 @@
       <c r="F12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="6"/>
+      <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -1060,13 +1073,13 @@
       <c r="F13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="6"/>
+      <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="21" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -1079,70 +1092,70 @@
       <c r="F14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="6"/>
+      <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="21" t="s">
+      <c r="B15" s="20"/>
+      <c r="C15" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="D15" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21" t="s">
+      <c r="E15" s="18"/>
+      <c r="F15" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="21"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+      <c r="G15" s="19"/>
+    </row>
+    <row r="16" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15" t="s">
+      <c r="E16" s="12"/>
+      <c r="F16" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="G16" s="15" t="s">
+      <c r="G16" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="H16" s="18" t="s">
+      <c r="H16" s="15" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+    <row r="17" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15" t="s">
+      <c r="E17" s="12"/>
+      <c r="F17" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="G17" s="15" t="s">
+      <c r="G17" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="H17" s="15" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1163,45 +1176,49 @@
       <c r="F18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="3"/>
+      <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" s="19"/>
-    </row>
-    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="E19" s="16"/>
+      <c r="F19" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="17"/>
+    </row>
+    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="3"/>
+      <c r="E20" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -1218,7 +1235,7 @@
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
+      <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
@@ -1231,7 +1248,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
+      <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
@@ -1248,24 +1265,43 @@
       <c r="F23" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="10"/>
-    </row>
-    <row r="24" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="11" t="s">
+      <c r="G23" s="9"/>
+    </row>
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13" t="s">
+      <c r="C24" s="24"/>
+      <c r="D24" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24" s="13"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="23"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>